<commit_message>
FSD-CPS: [Selenium] Update user register test with additional phone input
</commit_message>
<xml_diff>
--- a/Capstone/foodBox/selenium/test-data.xlsx
+++ b/Capstone/foodBox/selenium/test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Git\yokekhei\simplilearn_fsd_projects\Capstone\foodBox\selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF4D467-4CDB-4E78-8008-944E5724A4FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F976BD11-09F4-48A9-8F87-75EB1056BC3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C4B8E351-14D4-46D5-AD9A-31B79C71B9C7}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{C4B8E351-14D4-46D5-AD9A-31B79C71B9C7}"/>
   </bookViews>
   <sheets>
     <sheet name="user-register" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>chrome</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Shah Alam</t>
+  </si>
+  <si>
+    <t>+60-125195864</t>
+  </si>
+  <si>
+    <t>+60-168710732</t>
   </si>
 </sst>
 </file>
@@ -105,10 +111,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -424,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{597AA67E-FAA6-44A7-8EC3-F039E6C7DC99}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,9 +443,10 @@
     <col min="4" max="4" width="21.140625" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,8 +468,11 @@
       <c r="G1" s="2">
         <v>47180</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -482,6 +493,9 @@
       </c>
       <c r="G2" s="2">
         <v>41060</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>